<commit_message>
Changes made to projectdata & projectQueries
</commit_message>
<xml_diff>
--- a/Generate SQL/attachments/RECEIPT.xlsx
+++ b/Generate SQL/attachments/RECEIPT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fharookshaik\Desktop\PythonApiTutorial\attachments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fharookshaik\Desktop\V Sem\DBMS\DBMS-Project Vehicle Insurance\Generate SQL\attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFA80EF-07FE-4B8D-AF81-D93926171C9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97056EA-58DD-44C9-8677-406775B9628A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6048" yWindow="3300" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="672" yWindow="636" windowWidth="21576" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,7 +443,8 @@
     <col min="2" max="2" width="23.21875" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.5546875" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -887,40 +888,6 @@
       </c>
       <c r="E26">
         <v>2025</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>2926</v>
-      </c>
-      <c r="B27" s="1">
-        <v>44055</v>
-      </c>
-      <c r="C27">
-        <v>1000</v>
-      </c>
-      <c r="D27">
-        <v>2726</v>
-      </c>
-      <c r="E27">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>2927</v>
-      </c>
-      <c r="B28" s="1">
-        <v>44057</v>
-      </c>
-      <c r="C28">
-        <v>5500</v>
-      </c>
-      <c r="D28">
-        <v>2727</v>
-      </c>
-      <c r="E28">
-        <v>2020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>